<commit_message>
time function for prioritizer needs to be fixed
</commit_message>
<xml_diff>
--- a/input_files/WGUPS Distance Table.xlsx
+++ b/input_files/WGUPS Distance Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\wgu_projects\c950\nhp3Task1\project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\wgu_projects\c950_final\wgups\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F2FDD7-1A59-4FD5-8600-FE1D7A01D584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C4357B-3D66-4C09-B650-F71C41D51974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14685" yWindow="-3840" windowWidth="12150" windowHeight="20835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>Western Governors University
 4001 South 700 East, 
@@ -243,7 +243,10 @@
 (84121)</t>
   </si>
   <si>
-    <t>DISTANCE BETWEEN HUBS IN MILES</t>
+    <t>hub_name</t>
+  </si>
+  <si>
+    <t>hub_address</t>
   </si>
 </sst>
 </file>
@@ -868,7 +871,7 @@
   <dimension ref="A1:AC28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:XFD7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +886,9 @@
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="19" t="s">
+        <v>55</v>
+      </c>
       <c r="C1" s="20" t="s">
         <v>0</v>
       </c>
@@ -2674,15 +2679,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="51" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dca2bb0f68bdf94cc5f80c9292ca56b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4cb8629785915e947a4406c57312ba8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3192,6 +3188,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3242,14 +3247,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{346B5534-CC83-47DD-8523-BB97FB1B43B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3265,6 +3262,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>